<commit_message>
Revert "Merge branch 'main' of https://github.com/AndreyOliveira0/LeitorArquivos-Vue"
This reverts commit 91ed4b6582bf0b60654653bfb8c29d9637ec0e21, reversing
changes made to a181e18279bac2e22aaadc21d123dab764e08e3f.
</commit_message>
<xml_diff>
--- a/src/frontend/components/sheets/Lista_Exemplo.xlsx
+++ b/src/frontend/components/sheets/Lista_Exemplo.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\AndreyOliveira0\LeitorArquivos-Vue\src\frontend\components\sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrey\Desktop\Nova pasta\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Disciplinas" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="118">
   <si>
     <t>Disciplina</t>
   </si>
@@ -381,37 +381,13 @@
   </si>
   <si>
     <t>Estagiario</t>
-  </si>
-  <si>
-    <t>D001</t>
-  </si>
-  <si>
-    <t>D002</t>
-  </si>
-  <si>
-    <t>D003</t>
-  </si>
-  <si>
-    <t>D004</t>
-  </si>
-  <si>
-    <t>D005</t>
-  </si>
-  <si>
-    <t>D006</t>
-  </si>
-  <si>
-    <t>D007</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -431,13 +407,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -475,36 +444,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Vírgula" xfId="2" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -785,22 +740,22 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
     <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="19" style="9" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="18" style="3" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1"/>
     <col min="11" max="11" width="17.42578125" customWidth="1"/>
     <col min="12" max="12" width="16.85546875" customWidth="1"/>
     <col min="13" max="13" width="10.85546875" customWidth="1"/>
@@ -832,263 +787,263 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
         <v>45698</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
         <v>45838</v>
       </c>
       <c r="F2" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2">
         <v>3</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
         <v>45698</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <v>45838</v>
       </c>
       <c r="F3" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3">
         <v>2</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2">
         <v>45698</v>
       </c>
-      <c r="E4" s="1">
-        <v>45838.5</v>
+      <c r="E4" s="2">
+        <v>45838</v>
       </c>
       <c r="F4" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4">
         <v>4</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2">
         <v>45705</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="2">
         <v>45833</v>
       </c>
       <c r="F5" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5">
         <v>6</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2">
         <v>45700</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="2">
         <v>45836</v>
       </c>
       <c r="F6" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6">
         <v>3</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D7" s="1">
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2">
         <v>45703</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="2">
         <v>45838</v>
       </c>
       <c r="F7" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7">
         <v>5</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" t="s">
         <v>38</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2">
         <v>45699</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="2">
         <v>45837</v>
       </c>
       <c r="F8" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8">
         <v>5</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="4"/>
+      <c r="C18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1101,397 +1056,397 @@
   <sheetPr codeName="Planilha2"/>
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15" style="3" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2">
         <v>40</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="2">
         <v>45720</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="2">
         <v>45836</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3">
         <v>35</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="2">
         <v>45720</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="2">
         <v>45836</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" t="s">
         <v>68</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4">
         <v>30</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="2">
         <v>45720</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="2">
         <v>45836</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" t="s">
         <v>83</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>72</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5">
         <v>40</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="2">
         <v>45720</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="2">
         <v>45836</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" t="s">
         <v>73</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>75</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" t="s">
         <v>67</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6">
         <v>25</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="2">
         <v>45720</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="2">
         <v>45836</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" t="s">
         <v>76</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7">
         <v>35</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="2">
         <v>45720</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="2">
         <v>45836</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" t="s">
         <v>78</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8">
         <v>45</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="2">
         <v>45720</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="2">
         <v>45836</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" t="s">
         <v>80</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9">
         <v>40</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="2">
         <v>45720</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="2">
         <v>45836</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" t="s">
         <v>82</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10">
         <v>30</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="2">
         <v>45720</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="2">
         <v>45836</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" t="s">
         <v>85</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" t="s">
         <v>86</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11">
         <v>50</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="2">
         <v>45720</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="2">
         <v>45836</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" t="s">
         <v>87</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="I11" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" t="s">
         <v>88</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12">
         <v>38</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="2">
         <v>45720</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="2">
         <v>45836</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" t="s">
         <v>89</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" t="s">
         <v>91</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" t="s">
         <v>71</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13">
         <v>32</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="2">
         <v>45720</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="2">
         <v>45836</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" t="s">
         <v>90</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="I13" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1506,222 +1461,222 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19" style="3" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2">
         <v>20251234</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s">
         <v>94</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" t="s">
         <v>95</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="2">
         <v>37684</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="2">
         <v>45836</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" t="s">
         <v>104</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3">
         <v>20255789</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="2">
         <v>38300</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="2">
         <v>45832</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" t="s">
         <v>103</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4">
         <v>20249876</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s">
         <v>94</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s">
         <v>95</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="2">
         <v>37156</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="2">
         <v>45360</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" t="s">
         <v>105</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5">
         <v>20254985</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" t="s">
         <v>99</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" t="s">
         <v>110</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="2">
         <v>33257</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="2">
         <v>45839</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" t="s">
         <v>108</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" t="s">
         <v>109</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6">
         <v>20236254</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" t="s">
         <v>94</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="2">
         <v>37449</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="2">
         <v>44959</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" t="s">
         <v>112</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" t="s">
         <v>115</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7">
         <v>20232565</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="2">
         <v>35141</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="2">
         <v>45269</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1744,135 +1699,135 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="29.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17" style="3" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" style="9" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2">
         <v>20251234</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s">
         <v>95</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" t="s">
         <v>116</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="2">
         <v>45720</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="2">
         <v>45836</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2">
         <v>1</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3">
         <v>20236254</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" t="s">
         <v>117</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="2">
         <v>45716</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="2">
         <v>45839</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3">
         <v>2</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4">
         <v>20232565</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s">
         <v>117</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="2">
         <v>45116</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="2">
         <v>45253</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4">
         <v>0</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>